<commit_message>
eg2 1-48 73-136 169-264
</commit_message>
<xml_diff>
--- a/eg2.xlsx
+++ b/eg2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shiqing/Desktop/Lipschitz-System-ID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC38064C-59C4-0E42-AF04-94E51159F9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930AE6AB-06EF-B04E-BF39-81C7D1B9A5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="34560" windowHeight="19800" activeTab="2" xr2:uid="{624D5C9E-D399-6E42-9BAD-9829FF00FD61}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34560" windowHeight="19800" activeTab="5" xr2:uid="{624D5C9E-D399-6E42-9BAD-9829FF00FD61}"/>
   </bookViews>
   <sheets>
     <sheet name="Ours 0.25" sheetId="1" r:id="rId1"/>
@@ -2244,10 +2244,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C910F4E5-1871-5D44-A4D1-B4921F11A929}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2292,42 +2292,42 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B2">
-        <v>1.0141516923904399</v>
+        <v>0.50343608856201105</v>
       </c>
       <c r="C2">
-        <v>0.182354071658651</v>
+        <v>2.1766328506469699</v>
       </c>
       <c r="D2">
-        <v>0.18012873076324101</v>
+        <v>2.1835943566765699</v>
       </c>
       <c r="E2">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="J2">
         <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-2)*4,0,4,1))</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K2">
         <f t="shared" ref="K2:O9" ca="1" si="0">AVERAGE(OFFSET(B$2,(ROW()-2)*4,0,4,1))</f>
-        <v>1.0141516923904399</v>
+        <v>0.50343608856201105</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18183029610751875</v>
+        <v>2.1774129129886575</v>
       </c>
       <c r="M2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18052621878121225</v>
+        <v>2.18107405096102</v>
       </c>
       <c r="N2">
         <f t="shared" ca="1" si="0"/>
-        <v>66.5</v>
+        <v>50.5</v>
       </c>
       <c r="O2">
         <f t="shared" ca="1" si="0"/>
@@ -2336,42 +2336,42 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B3">
-        <v>1.0141516923904399</v>
+        <v>0.50343608856201105</v>
       </c>
       <c r="C3">
-        <v>0.17989082154222</v>
+        <v>2.1775262559890698</v>
       </c>
       <c r="D3">
-        <v>0.184625543513388</v>
+        <v>2.1808682247331901</v>
       </c>
       <c r="E3">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J9" ca="1" si="1">AVERAGE(OFFSET(A$2,(ROW()-2)*4,0,4,1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0283033847808798</v>
+        <v>1.0068721771240201</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6151730988772702E-3</v>
+        <v>3.5877577021717975E-2</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.52145578571867E-3</v>
+        <v>3.589527369447193E-2</v>
       </c>
       <c r="N3">
         <f t="shared" ca="1" si="0"/>
-        <v>70.5</v>
+        <v>54.5</v>
       </c>
       <c r="O3">
         <f t="shared" ca="1" si="0"/>
@@ -2380,174 +2380,174 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B4">
-        <v>1.0141516923904399</v>
+        <v>0.50343608856201105</v>
       </c>
       <c r="C4">
-        <v>0.181765205981607</v>
+        <v>2.1766223686218198</v>
       </c>
       <c r="D4">
-        <v>0.177050863445367</v>
+        <v>2.1836080429660201</v>
       </c>
       <c r="E4">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0137443542480402</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.44796273100655E-4</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.4843390178251203E-4</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>58.5</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.5</v>
+      </c>
+      <c r="B5">
+        <v>0.50343608856201105</v>
+      </c>
+      <c r="C5">
+        <v>2.17887017669677</v>
+      </c>
+      <c r="D5">
+        <v>2.1762255794683001</v>
+      </c>
+      <c r="E5">
+        <v>52</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="K4">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.0566067695617596</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.8580142772004444E-4</v>
-      </c>
-      <c r="M4">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.8844408656268316E-4</v>
-      </c>
-      <c r="N4">
-        <f t="shared" ca="1" si="0"/>
-        <v>74.5</v>
-      </c>
-      <c r="O4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1.0141516923904399</v>
-      </c>
-      <c r="C5">
-        <v>0.18331108524759701</v>
-      </c>
-      <c r="D5">
-        <v>0.18029973740285299</v>
-      </c>
-      <c r="E5">
-        <v>68</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="K5" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.0274887084960902</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.3488306086510364E-4</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.4031718390879576E-4</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>62.5</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1.0068721771240201</v>
+      </c>
+      <c r="C6">
+        <v>3.5592726659774698E-2</v>
+      </c>
+      <c r="D6">
+        <v>3.5595786431507702E-2</v>
+      </c>
+      <c r="E6">
+        <v>53</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="J6">
         <f t="shared" ca="1" si="1"/>
         <v>8</v>
       </c>
-      <c r="K5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.1132135391235298</v>
-      </c>
-      <c r="L5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.6951944898001202E-4</v>
-      </c>
-      <c r="M5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.7297403910988001E-4</v>
-      </c>
-      <c r="N5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>78.5</v>
-      </c>
-      <c r="O5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>2.0283033847808798</v>
-      </c>
-      <c r="C6">
-        <v>2.6262016776315701E-3</v>
-      </c>
-      <c r="D6">
-        <v>2.6302639612453501E-3</v>
-      </c>
-      <c r="E6">
-        <v>69</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="J6">
+      <c r="K6">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.0549774169921804</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.3306349304039005E-4</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.3853282588534003E-4</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ca="1" si="0"/>
+        <v>66.5</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1.0068721771240201</v>
+      </c>
+      <c r="C7">
+        <v>3.6501656001806201E-2</v>
+      </c>
+      <c r="D7">
+        <v>3.6691080304277902E-2</v>
+      </c>
+      <c r="E7">
+        <v>54</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="J7">
         <f t="shared" ca="1" si="1"/>
         <v>16</v>
       </c>
-      <c r="K6">
-        <f t="shared" ca="1" si="0"/>
-        <v>16.226427078246999</v>
-      </c>
-      <c r="L6">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.6626587132418429E-4</v>
-      </c>
-      <c r="M6">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.7168505963142301E-4</v>
-      </c>
-      <c r="N6">
-        <f t="shared" ca="1" si="0"/>
-        <v>82.5</v>
-      </c>
-      <c r="O6">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>2.0283033847808798</v>
-      </c>
-      <c r="C7">
-        <v>2.55994174435792E-3</v>
-      </c>
-      <c r="D7">
-        <v>2.6434074048357001E-3</v>
-      </c>
-      <c r="E7">
-        <v>70</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <f t="shared" ca="1" si="1"/>
-        <v>32</v>
-      </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>32.452854156494098</v>
+        <v>16.1099548339843</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6898660087939751E-4</v>
+        <v>5.3380343744065576E-4</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7348558670436954E-4</v>
+        <v>5.3837227743159025E-4</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="0"/>
-        <v>86.5</v>
+        <v>70.5</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="0"/>
@@ -2556,271 +2556,229 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>2.0283033847808798</v>
+        <v>1.0068721771240201</v>
       </c>
       <c r="C8">
-        <v>2.5954600772544502E-3</v>
+        <v>3.5614374345541003E-2</v>
       </c>
       <c r="D8">
-        <v>2.3384923598605998E-3</v>
+        <v>3.5849563279159502E-2</v>
       </c>
       <c r="E8">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="J8" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>64.905708312988196</v>
-      </c>
-      <c r="L8" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.6961259335832227E-4</v>
-      </c>
-      <c r="M8" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.7343222805735948E-4</v>
-      </c>
-      <c r="N8" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>90.5</v>
-      </c>
-      <c r="O8" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1.0068721771240201</v>
+      </c>
+      <c r="C9">
+        <v>3.5801551079749999E-2</v>
+      </c>
+      <c r="D9">
+        <v>3.5444664762942599E-2</v>
+      </c>
+      <c r="E9">
+        <v>56</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>2</v>
       </c>
-      <c r="B9">
-        <v>2.0283033847808798</v>
-      </c>
-      <c r="C9">
-        <v>2.6790888962651398E-3</v>
-      </c>
-      <c r="D9">
-        <v>2.4736594169330302E-3</v>
-      </c>
-      <c r="E9">
-        <v>72</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <f t="shared" ca="1" si="1"/>
-        <v>128</v>
-      </c>
-      <c r="K9">
-        <f t="shared" ca="1" si="0"/>
-        <v>129.81141662597599</v>
-      </c>
-      <c r="L9">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.7210625606970793E-4</v>
-      </c>
-      <c r="M9">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.7582962115290811E-4</v>
-      </c>
-      <c r="N9">
-        <f t="shared" ca="1" si="0"/>
-        <v>94.5</v>
-      </c>
-      <c r="O9">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>4.0566067695617596</v>
-      </c>
-      <c r="C10">
-        <v>5.9090811103776504E-4</v>
-      </c>
-      <c r="D10">
-        <v>5.9912694488511401E-4</v>
-      </c>
-      <c r="E10">
-        <v>73</v>
-      </c>
-      <c r="F10">
+      <c r="B10" s="2">
+        <v>2.0137443542480402</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5.4671502402052203E-4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5.5108411451890605E-4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>57</v>
+      </c>
+      <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="M10">
         <f ca="1">MIN(M2:M9)</f>
-        <v>5.7168505963142301E-4</v>
+        <v>5.3837227743159025E-4</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.0137443542480402</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5.41395342070609E-4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5.4446025213944396E-4</v>
+      </c>
+      <c r="E11" s="2">
+        <v>58</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.0137443542480402</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5.44865331286564E-4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5.5057641562181203E-4</v>
+      </c>
+      <c r="E12" s="2">
+        <v>59</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2.0137443542480402</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5.4620939502492496E-4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5.4761482484988596E-4</v>
+      </c>
+      <c r="E13" s="2">
+        <v>60</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>4</v>
       </c>
-      <c r="B11">
-        <v>4.0566067695617596</v>
-      </c>
-      <c r="C11">
-        <v>5.8026180419986999E-4</v>
-      </c>
-      <c r="D11">
-        <v>5.8439645129870895E-4</v>
-      </c>
-      <c r="E11">
-        <v>74</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="B14" s="4">
+        <v>4.0274887084960902</v>
+      </c>
+      <c r="C14" s="4">
+        <v>5.3520710361190096E-4</v>
+      </c>
+      <c r="D14" s="4">
+        <v>5.4482978755299703E-4</v>
+      </c>
+      <c r="E14" s="4">
+        <v>61</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
         <v>4</v>
       </c>
-      <c r="B12">
-        <v>4.0566067695617596</v>
-      </c>
-      <c r="C12">
-        <v>5.8405404386024495E-4</v>
-      </c>
-      <c r="D12">
-        <v>5.8256732058307103E-4</v>
-      </c>
-      <c r="E12">
-        <v>75</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="B15" s="4">
+        <v>4.0274887084960902</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5.3389373254030903E-4</v>
+      </c>
+      <c r="D15" s="4">
+        <v>5.3813045968266005E-4</v>
+      </c>
+      <c r="E15" s="4">
+        <v>62</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>4</v>
       </c>
-      <c r="B13">
-        <v>4.0566067695617596</v>
-      </c>
-      <c r="C13">
-        <v>5.8798175178229799E-4</v>
-      </c>
-      <c r="D13">
-        <v>5.8768562948383898E-4</v>
-      </c>
-      <c r="E13">
-        <v>76</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2">
-        <v>8.1132135391235298</v>
-      </c>
-      <c r="C14" s="2">
-        <v>5.7217467427849496E-4</v>
-      </c>
-      <c r="D14" s="2">
-        <v>5.7575543397896903E-4</v>
-      </c>
-      <c r="E14" s="2">
-        <v>77</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>8</v>
-      </c>
-      <c r="B15" s="2">
-        <v>8.1132135391235298</v>
-      </c>
-      <c r="C15" s="2">
-        <v>5.6563148973509604E-4</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5.6990910429103301E-4</v>
-      </c>
-      <c r="E15" s="2">
-        <v>78</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>8</v>
-      </c>
-      <c r="B16" s="2">
-        <v>8.1132135391235298</v>
-      </c>
-      <c r="C16" s="2">
-        <v>5.6951258325192299E-4</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5.7272411133865503E-4</v>
-      </c>
-      <c r="E16" s="2">
-        <v>79</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="B16" s="4">
+        <v>4.0274887084960902</v>
+      </c>
+      <c r="C16" s="4">
+        <v>5.3533195322379395E-4</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5.3911201472714497E-4</v>
+      </c>
+      <c r="E16" s="4">
+        <v>63</v>
+      </c>
+      <c r="F16" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>8</v>
-      </c>
-      <c r="B17" s="2">
-        <v>8.1132135391235298</v>
-      </c>
-      <c r="C17" s="2">
-        <v>5.7075904865453396E-4</v>
-      </c>
-      <c r="D17" s="2">
-        <v>5.7350750683086299E-4</v>
-      </c>
-      <c r="E17" s="2">
-        <v>80</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="A17" s="4">
+        <v>4</v>
+      </c>
+      <c r="B17" s="4">
+        <v>4.0274887084960902</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5.3509945408441095E-4</v>
+      </c>
+      <c r="D17" s="4">
+        <v>5.3919647367238097E-4</v>
+      </c>
+      <c r="E17" s="4">
+        <v>64</v>
+      </c>
+      <c r="F17" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B18" s="4">
-        <v>16.226427078246999</v>
+        <v>8.0549774169921804</v>
       </c>
       <c r="C18" s="4">
-        <v>5.6798992201551198E-4</v>
+        <v>5.3272665482945701E-4</v>
       </c>
       <c r="D18" s="4">
-        <v>5.7075067339816402E-4</v>
+        <v>5.4266521815435895E-4</v>
       </c>
       <c r="E18" s="4">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -2828,19 +2786,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B19" s="4">
-        <v>16.226427078246999</v>
+        <v>8.0549774169921804</v>
       </c>
       <c r="C19" s="4">
-        <v>5.66158735141449E-4</v>
+        <v>5.3388965432532099E-4</v>
       </c>
       <c r="D19" s="4">
-        <v>5.7288773005327402E-4</v>
+        <v>5.3793034304206204E-4</v>
       </c>
       <c r="E19" s="4">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
@@ -2848,19 +2806,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B20" s="4">
-        <v>16.226427078246999</v>
+        <v>8.0549774169921804</v>
       </c>
       <c r="C20" s="4">
-        <v>5.6385922480718805E-4</v>
+        <v>5.3282709205523099E-4</v>
       </c>
       <c r="D20" s="4">
-        <v>5.7121278621467201E-4</v>
+        <v>5.3707223180177199E-4</v>
       </c>
       <c r="E20" s="4">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
@@ -2868,19 +2826,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B21" s="4">
-        <v>16.226427078246999</v>
+        <v>8.0549774169921804</v>
       </c>
       <c r="C21" s="4">
-        <v>5.67055603332588E-4</v>
+        <v>5.32810570951551E-4</v>
       </c>
       <c r="D21" s="4">
-        <v>5.7188904885958197E-4</v>
+        <v>5.3646351054316703E-4</v>
       </c>
       <c r="E21" s="4">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
@@ -2888,19 +2846,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B22" s="4">
-        <v>32.452854156494098</v>
+        <v>16.1099548339843</v>
       </c>
       <c r="C22" s="4">
-        <v>5.7176252741805798E-4</v>
+        <v>5.3240928314626204E-4</v>
       </c>
       <c r="D22" s="4">
-        <v>5.7552236830815597E-4</v>
+        <v>5.4179476763145499E-4</v>
       </c>
       <c r="E22" s="4">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -2908,19 +2866,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B23" s="4">
-        <v>32.452854156494098</v>
+        <v>16.1099548339843</v>
       </c>
       <c r="C23" s="4">
-        <v>5.6737957972485798E-4</v>
+        <v>5.3358408650383299E-4</v>
       </c>
       <c r="D23" s="4">
-        <v>5.7364400654135003E-4</v>
+        <v>5.36472148448822E-4</v>
       </c>
       <c r="E23" s="4">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -2928,19 +2886,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B24" s="4">
-        <v>32.452854156494098</v>
+        <v>16.1099548339843</v>
       </c>
       <c r="C24" s="4">
-        <v>5.6918153483575097E-4</v>
+        <v>5.3274723063222998E-4</v>
       </c>
       <c r="D24" s="4">
-        <v>5.7355711513357003E-4</v>
+        <v>5.3596395738185595E-4</v>
       </c>
       <c r="E24" s="4">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -2948,183 +2906,55 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B25" s="4">
-        <v>32.452854156494098</v>
+        <v>16.1099548339843</v>
       </c>
       <c r="C25" s="4">
-        <v>5.6762276153892301E-4</v>
+        <v>5.3647314948029802E-4</v>
       </c>
       <c r="D25" s="4">
-        <v>5.7121885683440201E-4</v>
+        <v>5.3925823626422805E-4</v>
       </c>
       <c r="E25" s="4">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F25" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
-        <v>64</v>
-      </c>
-      <c r="B26" s="4">
-        <v>64.905708312988196</v>
-      </c>
-      <c r="C26" s="4">
-        <v>5.68279432782779E-4</v>
-      </c>
-      <c r="D26" s="4">
-        <v>5.7047968598539505E-4</v>
-      </c>
-      <c r="E26" s="4">
-        <v>89</v>
-      </c>
-      <c r="F26" s="4">
-        <v>1</v>
-      </c>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
-        <v>64</v>
-      </c>
-      <c r="B27" s="4">
-        <v>64.905708312988196</v>
-      </c>
-      <c r="C27" s="4">
-        <v>5.6790220672573604E-4</v>
-      </c>
-      <c r="D27" s="4">
-        <v>5.7500906954167995E-4</v>
-      </c>
-      <c r="E27" s="4">
-        <v>90</v>
-      </c>
-      <c r="F27" s="4">
-        <v>1</v>
-      </c>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>64</v>
-      </c>
-      <c r="B28" s="4">
-        <v>64.905708312988196</v>
-      </c>
-      <c r="C28" s="4">
-        <v>5.7340912069569095E-4</v>
-      </c>
-      <c r="D28" s="4">
-        <v>5.7523057440225496E-4</v>
-      </c>
-      <c r="E28" s="4">
-        <v>91</v>
-      </c>
-      <c r="F28" s="4">
-        <v>1</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
-        <v>64</v>
-      </c>
-      <c r="B29" s="4">
-        <v>64.905708312988196</v>
-      </c>
-      <c r="C29" s="4">
-        <v>5.6885961322908297E-4</v>
-      </c>
-      <c r="D29" s="4">
-        <v>5.7300958230010795E-4</v>
-      </c>
-      <c r="E29" s="4">
-        <v>92</v>
-      </c>
-      <c r="F29" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>128</v>
-      </c>
-      <c r="B30">
-        <v>129.81141662597599</v>
-      </c>
-      <c r="C30">
-        <v>5.6827455968430499E-4</v>
-      </c>
-      <c r="D30">
-        <v>5.7056505630618702E-4</v>
-      </c>
-      <c r="E30">
-        <v>93</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>128</v>
-      </c>
-      <c r="B31">
-        <v>129.81141662597599</v>
-      </c>
-      <c r="C31">
-        <v>5.6999718340861895E-4</v>
-      </c>
-      <c r="D31">
-        <v>5.7594825234703396E-4</v>
-      </c>
-      <c r="E31">
-        <v>94</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>128</v>
-      </c>
-      <c r="B32">
-        <v>129.81141662597599</v>
-      </c>
-      <c r="C32">
-        <v>5.7726450277143697E-4</v>
-      </c>
-      <c r="D32">
-        <v>5.7969049370478604E-4</v>
-      </c>
-      <c r="E32">
-        <v>95</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>128</v>
-      </c>
-      <c r="B33">
-        <v>129.81141662597599</v>
-      </c>
-      <c r="C33">
-        <v>5.7288877841447103E-4</v>
-      </c>
-      <c r="D33">
-        <v>5.7711468225362501E-4</v>
-      </c>
-      <c r="E33">
-        <v>96</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4708,8 +4538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D6121D-E5CF-1A48-8933-0BAD4C1790A9}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4750,63 +4580,57 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>1E-8</v>
       </c>
-      <c r="B2" s="2">
-        <v>6.0041419600613197E-4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>6.0144016455489896E-4</v>
-      </c>
-      <c r="D2" s="2">
-        <v>161</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>11.711</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="B2" s="4">
+        <v>5.41926246369257E-4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5.4944366914409901E-4</v>
+      </c>
+      <c r="D2" s="4">
+        <v>137</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5">
         <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-2)*4,0,4,1))</f>
         <v>1E-8</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <f t="shared" ref="K2:N9" ca="1" si="0">AVERAGE(OFFSET(B$2,(ROW()-2)*4,0,4,1))</f>
-        <v>6.1113358438991496E-4</v>
-      </c>
-      <c r="L2" s="7">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.1082911366302454E-4</v>
-      </c>
-      <c r="M2" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>162.5</v>
-      </c>
-      <c r="N2" s="3">
+        <v>5.4721664829412444E-4</v>
+      </c>
+      <c r="L2" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.5184196436089557E-4</v>
+      </c>
+      <c r="M2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>138.5</v>
+      </c>
+      <c r="N2" s="5">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>1E-8</v>
       </c>
-      <c r="B3" s="2">
-        <v>6.2069915727738702E-4</v>
-      </c>
-      <c r="C3" s="2">
-        <v>6.2034941577124097E-4</v>
-      </c>
-      <c r="D3" s="2">
-        <v>162</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>13.887</v>
+      <c r="B3" s="4">
+        <v>5.4839390292763695E-4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5.5113619128182797E-4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>138</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ref="J3:J9" ca="1" si="1">AVERAGE(OFFSET(A$2,(ROW()-2)*4,0,4,1))</f>
@@ -4814,15 +4638,15 @@
       </c>
       <c r="K3" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1009303094988494E-4</v>
+        <v>5.4662439271341951E-4</v>
       </c>
       <c r="L3" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1235278471425693E-4</v>
+        <v>5.5097479761205873E-4</v>
       </c>
       <c r="M3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>166.5</v>
+        <v>142.5</v>
       </c>
       <c r="N3" s="5">
         <f t="shared" ca="1" si="0"/>
@@ -4830,63 +4654,57 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="5">
         <v>1E-8</v>
       </c>
-      <c r="B4" s="2">
-        <v>6.1442296355035798E-4</v>
-      </c>
-      <c r="C4" s="2">
-        <v>6.1359601468726399E-4</v>
-      </c>
-      <c r="D4" s="2">
-        <v>163</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>15.571999999999999</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="B4" s="4">
+        <v>5.5013704607263195E-4</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5.5629565457629502E-4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>139</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
         <f t="shared" ca="1" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="K4" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.1089777218986706E-4</v>
-      </c>
-      <c r="L4" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.1244837885375417E-4</v>
-      </c>
-      <c r="M4" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>170.5</v>
-      </c>
-      <c r="N4" s="5">
+      <c r="K4" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.4678430308122128E-4</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.5093768420354803E-4</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>146.5</v>
+      </c>
+      <c r="N4" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="5">
         <v>1E-8</v>
       </c>
-      <c r="B5" s="2">
-        <v>6.0899802072578299E-4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>6.0793085963869401E-4</v>
-      </c>
-      <c r="D5" s="2">
-        <v>164</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>13.675000000000001</v>
+      <c r="B5" s="4">
+        <v>5.4840939780697196E-4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5.5049234244135996E-4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>140</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" ca="1" si="1"/>
@@ -4894,15 +4712,15 @@
       </c>
       <c r="K5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1374124696037392E-4</v>
+        <v>5.5187327221501575E-4</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1528938838922072E-4</v>
+        <v>5.5658835485788147E-4</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>174.5</v>
+        <v>150.5</v>
       </c>
       <c r="N5" s="5">
         <f t="shared" ca="1" si="0"/>
@@ -4914,13 +4732,13 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="B6" s="4">
-        <v>6.0671953804695999E-4</v>
+        <v>5.4299019603058698E-4</v>
       </c>
       <c r="C6" s="4">
-        <v>6.1044584024029795E-4</v>
+        <v>5.5131978973758098E-4</v>
       </c>
       <c r="D6" s="4">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
@@ -4932,15 +4750,15 @@
       </c>
       <c r="K6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6954505342799219E-4</v>
+        <v>5.7794446547049998E-4</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6713293075873394E-4</v>
+        <v>5.8176417858784701E-4</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>178.5</v>
+        <v>154.5</v>
       </c>
       <c r="N6" s="5">
         <f t="shared" ca="1" si="0"/>
@@ -4952,13 +4770,13 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="B7" s="4">
-        <v>6.1102821717868498E-4</v>
+        <v>5.4678227556869297E-4</v>
       </c>
       <c r="C7" s="4">
-        <v>6.1675184076862705E-4</v>
+        <v>5.4899573023579299E-4</v>
       </c>
       <c r="D7" s="4">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
@@ -4970,15 +4788,15 @@
       </c>
       <c r="K7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7733107005809833E-4</v>
+        <v>7.4878711584024083E-4</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6105509750624E-4</v>
+        <v>7.4920679617207421E-4</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>182.5</v>
+        <v>158.5</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" ca="1" si="0"/>
@@ -4990,13 +4808,13 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="B8" s="4">
-        <v>6.1980338537650603E-4</v>
+        <v>5.4677156819961902E-4</v>
       </c>
       <c r="C8" s="4">
-        <v>6.1879554853493395E-4</v>
+        <v>5.5187162969136795E-4</v>
       </c>
       <c r="D8" s="4">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -5008,15 +4826,15 @@
       </c>
       <c r="K8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.4788148409678095E-3</v>
+        <v>3.464594984706487E-3</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2534477532081222E-3</v>
+        <v>3.3366143976702972E-3</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>186.5</v>
+        <v>162.5</v>
       </c>
       <c r="N8" s="5">
         <f t="shared" ca="1" si="0"/>
@@ -5028,13 +4846,13 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="B9" s="4">
-        <v>6.0282098319738896E-4</v>
+        <v>5.4995353105477898E-4</v>
       </c>
       <c r="C9" s="4">
-        <v>6.0341790931316901E-4</v>
+        <v>5.51712040783493E-4</v>
       </c>
       <c r="D9" s="4">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -5046,15 +4864,15 @@
       </c>
       <c r="K9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95775334369633824</v>
+        <v>1.4517841141797583</v>
       </c>
       <c r="L9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93775767128352272</v>
+        <v>1.073173625643844</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>190.5</v>
+        <v>166.5</v>
       </c>
       <c r="N9" s="5">
         <f t="shared" ca="1" si="0"/>
@@ -5062,74 +4880,74 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="B10" s="4">
-        <v>6.0882785545675203E-4</v>
-      </c>
-      <c r="C10" s="4">
-        <v>6.1045092572282295E-4</v>
-      </c>
-      <c r="D10" s="4">
-        <v>169</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="B10" s="2">
+        <v>5.4344469686038702E-4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5.5203445542716405E-4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>145</v>
+      </c>
+      <c r="E10" s="2">
         <v>1</v>
       </c>
       <c r="L10">
         <f ca="1">MIN(L2:L9)</f>
-        <v>6.1082911366302454E-4</v>
+        <v>5.5093768420354803E-4</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="B11" s="4">
-        <v>6.1842446837252004E-4</v>
-      </c>
-      <c r="C11" s="4">
-        <v>6.2343241638099798E-4</v>
-      </c>
-      <c r="D11" s="4">
-        <v>170</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="B11" s="2">
+        <v>5.4675683104433103E-4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5.4808842351179601E-4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>146</v>
+      </c>
+      <c r="E11" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="B12" s="4">
-        <v>6.1882309581404605E-4</v>
-      </c>
-      <c r="C12" s="4">
-        <v>6.1897190786318204E-4</v>
-      </c>
-      <c r="D12" s="4">
-        <v>171</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="B12" s="2">
+        <v>5.4924231246113696E-4</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5.5396067965508703E-4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>147</v>
+      </c>
+      <c r="E12" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="B13" s="4">
-        <v>5.9751566911615003E-4</v>
-      </c>
-      <c r="C13" s="4">
-        <v>5.9693826544801403E-4</v>
-      </c>
-      <c r="D13" s="4">
-        <v>172</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="B13" s="2">
+        <v>5.4769337195903001E-4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5.4966717822014502E-4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>148</v>
+      </c>
+      <c r="E13" s="2">
         <v>1</v>
       </c>
     </row>
@@ -5138,13 +4956,13 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="B14">
-        <v>6.1082480912829501E-4</v>
+        <v>5.4969457532279102E-4</v>
       </c>
       <c r="C14">
-        <v>6.1503354732368905E-4</v>
+        <v>5.5699890248097803E-4</v>
       </c>
       <c r="D14">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -5155,13 +4973,13 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="B15">
-        <v>6.1185607839468401E-4</v>
+        <v>5.5122252376750103E-4</v>
       </c>
       <c r="C15">
-        <v>6.1564046103190903E-4</v>
+        <v>5.5241879449481005E-4</v>
       </c>
       <c r="D15">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -5172,13 +4990,13 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="B16">
-        <v>6.2753468000449196E-4</v>
+        <v>5.55050844559446E-4</v>
       </c>
       <c r="C16">
-        <v>6.2554147762228804E-4</v>
+        <v>5.6302289079554404E-4</v>
       </c>
       <c r="D16">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -5189,13 +5007,13 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="B17">
-        <v>6.0474942031402503E-4</v>
+        <v>5.5152514521032497E-4</v>
       </c>
       <c r="C17">
-        <v>6.04942067578997E-4</v>
+        <v>5.5391283166019399E-4</v>
       </c>
       <c r="D17">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -5206,13 +5024,13 @@
         <v>1E-4</v>
       </c>
       <c r="B18">
-        <v>6.6319399226955598E-4</v>
+        <v>5.7868409161455903E-4</v>
       </c>
       <c r="C18">
-        <v>6.7641262518558303E-4</v>
+        <v>5.8366856066907505E-4</v>
       </c>
       <c r="D18">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -5223,13 +5041,13 @@
         <v>1E-4</v>
       </c>
       <c r="B19">
-        <v>6.58737985892839E-4</v>
+        <v>5.7505093975923898E-4</v>
       </c>
       <c r="C19">
-        <v>6.5660282018383496E-4</v>
+        <v>5.7272240741973197E-4</v>
       </c>
       <c r="D19">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -5240,13 +5058,13 @@
         <v>1E-4</v>
       </c>
       <c r="B20">
-        <v>6.8931868084666601E-4</v>
+        <v>5.8041596319526403E-4</v>
       </c>
       <c r="C20">
-        <v>6.7292798402771904E-4</v>
+        <v>5.8937194304107697E-4</v>
       </c>
       <c r="D20">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -5257,13 +5075,13 @@
         <v>1E-4</v>
       </c>
       <c r="B21">
-        <v>6.6692955470290798E-4</v>
+        <v>5.7762686731293797E-4</v>
       </c>
       <c r="C21">
-        <v>6.6258829363779895E-4</v>
+        <v>5.8129380322150404E-4</v>
       </c>
       <c r="D21">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -5274,13 +5092,13 @@
         <v>1E-3</v>
       </c>
       <c r="B22">
-        <v>9.31884528891408E-4</v>
+        <v>7.5570705803111105E-4</v>
       </c>
       <c r="C22">
-        <v>9.4429495852036403E-4</v>
+        <v>7.5359870998521002E-4</v>
       </c>
       <c r="D22">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -5291,13 +5109,13 @@
         <v>1E-3</v>
       </c>
       <c r="B23">
-        <v>9.88194873165869E-4</v>
+        <v>7.3320005889981898E-4</v>
       </c>
       <c r="C23">
-        <v>1.0055391785671101E-3</v>
+        <v>7.1736435876020195E-4</v>
       </c>
       <c r="D23">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -5308,13 +5126,13 @@
         <v>1E-3</v>
       </c>
       <c r="B24">
-        <v>9.8992244564482298E-4</v>
+        <v>7.5610822103917602E-4</v>
       </c>
       <c r="C24">
-        <v>9.3182174923812098E-4</v>
+        <v>7.8136392069719403E-4</v>
       </c>
       <c r="D24">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -5325,13 +5143,13 @@
         <v>1E-3</v>
       </c>
       <c r="B25">
-        <v>9.9932243253029302E-4</v>
+        <v>7.5013312539085704E-4</v>
       </c>
       <c r="C25">
-        <v>9.6256450369936505E-4</v>
+        <v>7.4450019524569097E-4</v>
       </c>
       <c r="D25">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -5342,13 +5160,13 @@
         <v>0.01</v>
       </c>
       <c r="B26">
-        <v>5.5974833206582503E-3</v>
+        <v>3.4582590067759101E-3</v>
       </c>
       <c r="C26">
-        <v>5.79402166778959E-3</v>
+        <v>3.4015328233326001E-3</v>
       </c>
       <c r="D26">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -5359,13 +5177,13 @@
         <v>0.01</v>
       </c>
       <c r="B27">
-        <v>5.09926428388301E-3</v>
+        <v>3.43492303136736E-3</v>
       </c>
       <c r="C27">
-        <v>4.9462787826756397E-3</v>
+        <v>3.1165065656113501E-3</v>
       </c>
       <c r="D27">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -5376,13 +5194,13 @@
         <v>0.01</v>
       </c>
       <c r="B28">
-        <v>5.4447425207149597E-3</v>
+        <v>3.5513509649783299E-3</v>
       </c>
       <c r="C28">
-        <v>5.0669391156297197E-3</v>
+        <v>3.4254438467738999E-3</v>
       </c>
       <c r="D28">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -5393,13 +5211,13 @@
         <v>0.01</v>
       </c>
       <c r="B29">
-        <v>5.7737692386150199E-3</v>
+        <v>3.4138469357043498E-3</v>
       </c>
       <c r="C29">
-        <v>5.2065514467375404E-3</v>
+        <v>3.40297435496334E-3</v>
       </c>
       <c r="D29">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -5410,13 +5228,13 @@
         <v>0.1</v>
       </c>
       <c r="B30">
-        <v>7.9303193387191398E-2</v>
+        <v>3.4631295219063697E-2</v>
       </c>
       <c r="C30">
-        <v>7.6216881919019597E-2</v>
+        <v>3.2619364168139001E-2</v>
       </c>
       <c r="D30">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -5427,13 +5245,13 @@
         <v>0.1</v>
       </c>
       <c r="B31">
-        <v>3.6042677644304701</v>
+        <v>3.4280919279158099E-2</v>
       </c>
       <c r="C31">
-        <v>3.5316734268980201</v>
+        <v>2.6455554102731298E-2</v>
       </c>
       <c r="D31">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -5444,13 +5262,13 @@
         <v>0.1</v>
       </c>
       <c r="B32">
-        <v>7.6917742387837398E-2</v>
+        <v>5.70629115829467</v>
       </c>
       <c r="C32">
-        <v>7.2686749949770105E-2</v>
+        <v>4.2035867864159204</v>
       </c>
       <c r="D32">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -5461,13 +5279,13 @@
         <v>0.1</v>
       </c>
       <c r="B33">
-        <v>7.0524674579854202E-2</v>
+        <v>3.1933083926141199E-2</v>
       </c>
       <c r="C33">
-        <v>7.0453626367281003E-2</v>
+        <v>3.0032797888585702E-2</v>
       </c>
       <c r="D33">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="E33">
         <v>1</v>

</xml_diff>